<commit_message>
Published state of ETDataset on 30 March 2016
</commit_message>
<xml_diff>
--- a/carriers_source_analyses/bio_ethanol.carrier.xlsx
+++ b/carriers_source_analyses/bio_ethanol.carrier.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="38400" windowHeight="23520" tabRatio="762" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="762" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Cover sheet" sheetId="14" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="202">
   <si>
     <t>Source</t>
   </si>
@@ -507,9 +507,6 @@
   </si>
   <si>
     <t>This sheet summarizes the Fuel Chain Emissions attributes formatted in the way they are used by the Energy Transition Model. These FCE are only specified for carriers and at the moment only for NL.</t>
-  </si>
-  <si>
-    <t>N.B. These FCE attributes have to be exported to ETSource manually as this is not automated yet.</t>
   </si>
   <si>
     <t>http://www.biotanken.nl/brandstoffen/bioethanol.html</t>
@@ -724,6 +721,56 @@
   <si>
     <t>Euro-super 95(I) excl tax</t>
   </si>
+  <si>
+    <r>
+      <t>from sugar</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>beets</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>from sugar</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cane</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -741,12 +788,19 @@
     <numFmt numFmtId="172" formatCode="0.00000000000"/>
     <numFmt numFmtId="173" formatCode="0.00000000000000"/>
   </numFmts>
-  <fonts count="47" x14ac:knownFonts="1">
+  <fonts count="48" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Lettertype hoofdtekst"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1546,760 +1600,761 @@
   </borders>
   <cellStyleXfs count="358">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="241">
+  <cellXfs count="242">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="17" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="18" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="13" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="13" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="23" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="23" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="24" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="23" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="24" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="23" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="183" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="49" fontId="23" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="17" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="183" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="12" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="12" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="12" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="22" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="22" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="23" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="22" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="23" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="13" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="27" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="13" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="22" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="183" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="49" fontId="22" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
     </xf>
-    <xf numFmtId="2" fontId="16" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="31" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="183" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="183" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="167" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="183" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="183" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="11" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="36" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="36" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" xfId="183" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="39" fillId="15" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="40" fillId="16" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="40" fillId="16" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
+    <xf numFmtId="166" fontId="25" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="14" fontId="41" fillId="16" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="169" fontId="25" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
+    <xf numFmtId="49" fontId="43" fillId="18" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="3" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="3" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="3" fontId="11" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="11" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="12" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="26" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="12" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="30" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="30" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="183" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="183" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="167" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="183" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="35" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="35" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" xfId="183" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="38" fillId="15" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="16" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="42" fillId="18" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="16" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="24" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="14" fontId="40" fillId="16" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="24" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="42" fillId="18" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="41" fillId="18" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="170" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="170" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="172" fontId="12" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="12" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="44" fillId="16" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="44" fillId="16" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="13" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="173" fontId="13" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="45" fillId="16" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="45" fillId="16" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="44" fillId="16" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="46" fillId="16" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="45" fillId="16" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="46" fillId="16" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="47" fillId="16" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="17" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="41" fillId="17" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="40" fillId="17" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="41" fillId="17" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="40" fillId="17" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="41" fillId="17" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="358">
@@ -2671,6 +2726,10 @@
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Button" lockText="1"/>
 </file>
 
+<file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Button" lockText="1"/>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -2679,14 +2738,14 @@
         <xdr:from>
           <xdr:col>6</xdr:col>
           <xdr:colOff>165100</xdr:colOff>
-          <xdr:row>2</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
+          <xdr:row>1</xdr:row>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>6</xdr:col>
           <xdr:colOff>3949700</xdr:colOff>
-          <xdr:row>3</xdr:row>
-          <xdr:rowOff>12700</xdr:rowOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>25400</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2725,6 +2784,67 @@
                   <a:cs typeface="Lucida Grande"/>
                 </a:rPr>
                 <a:t>Update carrier attributes on ETSource</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData fPrintsWithSheet="0"/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>165100</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>177800</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>3949700</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2051" name="export_fce" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2051"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="27432" bIns="22860" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Lucida Grande"/>
+                  <a:ea typeface="Lucida Grande"/>
+                  <a:cs typeface="Lucida Grande"/>
+                </a:rPr>
+                <a:t>Update FCE attributes on ETSource (next sheet)</a:t>
               </a:r>
             </a:p>
           </xdr:txBody>
@@ -3919,6 +4039,7 @@
     </sheetNames>
     <definedNames>
       <definedName name="update_attributes"/>
+      <definedName name="update_fce"/>
     </definedNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
@@ -4446,7 +4567,7 @@
     </row>
     <row r="27" spans="1:4">
       <c r="B27" s="20" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C27" s="212">
         <v>42227</v>
@@ -4454,17 +4575,17 @@
     </row>
     <row r="28" spans="1:4">
       <c r="C28" s="211" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="C29" s="211" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="C30" s="211" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -4509,28 +4630,28 @@
       <c r="G1" s="36"/>
     </row>
     <row r="2" spans="2:11" ht="15" customHeight="1">
-      <c r="B2" s="219" t="s">
+      <c r="B2" s="228" t="s">
         <v>145</v>
       </c>
-      <c r="C2" s="220"/>
-      <c r="D2" s="220"/>
-      <c r="E2" s="221"/>
+      <c r="C2" s="229"/>
+      <c r="D2" s="229"/>
+      <c r="E2" s="230"/>
       <c r="F2" s="36"/>
       <c r="G2" s="36"/>
     </row>
     <row r="3" spans="2:11">
-      <c r="B3" s="222"/>
-      <c r="C3" s="223"/>
-      <c r="D3" s="223"/>
-      <c r="E3" s="224"/>
+      <c r="B3" s="231"/>
+      <c r="C3" s="232"/>
+      <c r="D3" s="232"/>
+      <c r="E3" s="233"/>
       <c r="F3" s="36"/>
       <c r="G3" s="36"/>
     </row>
     <row r="4" spans="2:11">
-      <c r="B4" s="225"/>
-      <c r="C4" s="226"/>
-      <c r="D4" s="226"/>
-      <c r="E4" s="227"/>
+      <c r="B4" s="234"/>
+      <c r="C4" s="235"/>
+      <c r="D4" s="235"/>
+      <c r="E4" s="236"/>
       <c r="F4" s="36"/>
       <c r="G4" s="36"/>
     </row>
@@ -4631,7 +4752,7 @@
       <c r="G11" s="132"/>
       <c r="H11" s="32"/>
       <c r="I11" s="217" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J11" s="46"/>
     </row>
@@ -4728,14 +4849,37 @@
                   <from>
                     <xdr:col>6</xdr:col>
                     <xdr:colOff>165100</xdr:colOff>
-                    <xdr:row>2</xdr:row>
-                    <xdr:rowOff>0</xdr:rowOff>
+                    <xdr:row>1</xdr:row>
+                    <xdr:rowOff>12700</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>6</xdr:col>
                     <xdr:colOff>3949700</xdr:colOff>
-                    <xdr:row>3</xdr:row>
-                    <xdr:rowOff>12700</xdr:rowOff>
+                    <xdr:row>2</xdr:row>
+                    <xdr:rowOff>25400</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+          <mc:Fallback/>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2051" r:id="rId4" name="export_fce">
+              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[2]!update_fce">
+                <anchor moveWithCells="1" sizeWithCells="1">
+                  <from>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>165100</xdr:colOff>
+                    <xdr:row>2</xdr:row>
+                    <xdr:rowOff>177800</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>3949700</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4786,29 +4930,27 @@
       <c r="G1" s="36"/>
     </row>
     <row r="2" spans="2:10" ht="15" customHeight="1">
-      <c r="B2" s="219" t="s">
+      <c r="B2" s="228" t="s">
         <v>146</v>
       </c>
-      <c r="C2" s="220"/>
-      <c r="D2" s="220"/>
-      <c r="E2" s="228"/>
+      <c r="C2" s="229"/>
+      <c r="D2" s="229"/>
+      <c r="E2" s="237"/>
       <c r="F2" s="36"/>
     </row>
     <row r="3" spans="2:10">
-      <c r="B3" s="222"/>
-      <c r="C3" s="223"/>
-      <c r="D3" s="223"/>
-      <c r="E3" s="229"/>
+      <c r="B3" s="231"/>
+      <c r="C3" s="232"/>
+      <c r="D3" s="232"/>
+      <c r="E3" s="238"/>
       <c r="F3" s="36"/>
       <c r="G3" s="36"/>
     </row>
     <row r="4" spans="2:10">
-      <c r="B4" s="230" t="s">
-        <v>147</v>
-      </c>
-      <c r="C4" s="231"/>
-      <c r="D4" s="231"/>
-      <c r="E4" s="232"/>
+      <c r="B4" s="239"/>
+      <c r="C4" s="240"/>
+      <c r="D4" s="240"/>
+      <c r="E4" s="241"/>
       <c r="F4" s="36"/>
       <c r="G4" s="36"/>
     </row>
@@ -4873,8 +5015,8 @@
     </row>
     <row r="10" spans="2:10" ht="16" thickBot="1">
       <c r="B10" s="41"/>
-      <c r="C10" s="132" t="s">
-        <v>46</v>
+      <c r="C10" s="227" t="s">
+        <v>200</v>
       </c>
       <c r="D10" s="132"/>
       <c r="E10" s="132"/>
@@ -5051,8 +5193,8 @@
     </row>
     <row r="19" spans="2:10" ht="16" thickBot="1">
       <c r="B19" s="41"/>
-      <c r="C19" s="132" t="s">
-        <v>59</v>
+      <c r="C19" s="227" t="s">
+        <v>201</v>
       </c>
       <c r="D19" s="132"/>
       <c r="E19" s="132"/>
@@ -5321,7 +5463,7 @@
       </c>
       <c r="N3" s="69"/>
       <c r="O3" s="69" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="P3" s="69"/>
       <c r="Q3" s="1" t="s">
@@ -5425,7 +5567,7 @@
       </c>
       <c r="P7" s="16"/>
       <c r="Q7" s="214" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="8" spans="2:17" s="6" customFormat="1" ht="16" thickBot="1">
@@ -6565,7 +6707,7 @@
       <c r="D7" s="140"/>
       <c r="E7" s="140"/>
       <c r="F7" s="140" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G7" s="140"/>
       <c r="H7" s="140"/>
@@ -6773,7 +6915,7 @@
       <c r="D14" s="140"/>
       <c r="E14" s="140"/>
       <c r="F14" s="140" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G14" s="140"/>
       <c r="H14" s="140"/>
@@ -6957,7 +7099,7 @@
       <c r="D20" s="140"/>
       <c r="E20" s="140"/>
       <c r="F20" s="140" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G20" s="140"/>
       <c r="H20" s="140"/>
@@ -7015,7 +7157,7 @@
       </c>
       <c r="G22" s="140"/>
       <c r="H22" s="140" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I22" s="140"/>
       <c r="J22" s="140"/>
@@ -7046,7 +7188,7 @@
       </c>
       <c r="G23" s="140"/>
       <c r="H23" s="140" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I23" s="140"/>
       <c r="J23" s="140"/>
@@ -7079,7 +7221,7 @@
         <v>73</v>
       </c>
       <c r="H24" s="140" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I24" s="140"/>
       <c r="J24" s="140"/>
@@ -7160,10 +7302,10 @@
         <v>1</v>
       </c>
       <c r="G27" s="154" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H27" s="155" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I27" s="140"/>
       <c r="J27" s="140"/>
@@ -7188,16 +7330,16 @@
       <c r="C28" s="140"/>
       <c r="D28" s="140"/>
       <c r="E28" s="159" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F28" s="157">
         <v>0.15</v>
       </c>
       <c r="G28" s="157" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H28" s="158" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I28" s="140"/>
       <c r="J28" s="140"/>
@@ -7220,33 +7362,33 @@
     <row r="29" spans="2:25" customFormat="1" ht="16">
       <c r="B29" s="127"/>
       <c r="E29" s="159" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F29" s="157">
         <f>F28*F18</f>
         <v>4.8276000000000003</v>
       </c>
       <c r="G29" s="157" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H29" s="158" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="30" spans="2:25" customFormat="1" ht="16">
       <c r="B30" s="127"/>
       <c r="E30" s="159" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F30" s="157">
         <f>F28*F17</f>
         <v>0.11175</v>
       </c>
       <c r="G30" s="157" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H30" s="158" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="31" spans="2:25" customFormat="1" ht="16">
@@ -7259,49 +7401,49 @@
     <row r="32" spans="2:25" customFormat="1" ht="16">
       <c r="B32" s="127"/>
       <c r="E32" s="159" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F32" s="157">
         <f>1-F28</f>
         <v>0.85</v>
       </c>
       <c r="G32" s="157" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H32" s="158" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="33" spans="2:8" customFormat="1" ht="16">
       <c r="B33" s="127"/>
       <c r="E33" s="159" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F33" s="157">
         <f>F32*F11</f>
         <v>18.087320000000002</v>
       </c>
       <c r="G33" s="157" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H33" s="158" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="34" spans="2:8" customFormat="1" ht="16">
       <c r="B34" s="127"/>
       <c r="E34" s="159" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F34" s="157">
         <f>F32*F10</f>
         <v>0.67490000000000006</v>
       </c>
       <c r="G34" s="157" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H34" s="158" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="35" spans="2:8" customFormat="1" ht="16">
@@ -7314,33 +7456,33 @@
     <row r="36" spans="2:8" customFormat="1" ht="16">
       <c r="B36" s="127"/>
       <c r="E36" s="159" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F36" s="157">
         <f>F30+F34</f>
         <v>0.78665000000000007</v>
       </c>
       <c r="G36" s="157" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H36" s="158" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="37" spans="2:8" customFormat="1" ht="16">
       <c r="B37" s="127"/>
       <c r="E37" s="159" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F37" s="157">
         <f>F29+F33</f>
         <v>22.914920000000002</v>
       </c>
       <c r="G37" s="157" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H37" s="158" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="38" spans="2:8" customFormat="1" ht="16">
@@ -7354,7 +7496,7 @@
         <v>61</v>
       </c>
       <c r="H38" s="158" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="39" spans="2:8" customFormat="1" ht="16">
@@ -15889,7 +16031,7 @@
       <c r="A515" s="187"/>
       <c r="B515" s="188"/>
       <c r="C515" s="185" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D515" s="140"/>
       <c r="E515" s="140"/>
@@ -15918,7 +16060,7 @@
       <c r="A516" s="187"/>
       <c r="B516" s="188"/>
       <c r="C516" s="189" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D516" s="140"/>
       <c r="E516" s="140"/>
@@ -15975,7 +16117,7 @@
       <c r="B518" s="188"/>
       <c r="C518" s="140"/>
       <c r="D518" s="140" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E518" s="140"/>
       <c r="F518" s="140"/>
@@ -16009,17 +16151,17 @@
       <c r="E519" s="187"/>
       <c r="F519" s="140"/>
       <c r="G519" s="140"/>
-      <c r="H519" s="233" t="s">
+      <c r="H519" s="219" t="s">
+        <v>155</v>
+      </c>
+      <c r="I519" s="220" t="s">
         <v>156</v>
       </c>
-      <c r="I519" s="234" t="s">
-        <v>157</v>
-      </c>
-      <c r="J519" s="235" t="s">
-        <v>200</v>
+      <c r="J519" s="221" t="s">
+        <v>199</v>
       </c>
       <c r="K519" s="196" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="L519" s="140"/>
       <c r="M519" s="140"/>
@@ -16038,18 +16180,18 @@
       <c r="B520" s="188"/>
       <c r="C520" s="140"/>
       <c r="D520" s="140" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E520" s="187"/>
       <c r="F520" s="140"/>
       <c r="G520" s="140"/>
       <c r="H520" s="191"/>
       <c r="I520" s="192"/>
-      <c r="J520" s="236" t="s">
-        <v>158</v>
+      <c r="J520" s="222" t="s">
+        <v>157</v>
       </c>
       <c r="K520" s="197" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="L520" s="140"/>
       <c r="M520" s="140"/>
@@ -16069,25 +16211,25 @@
       <c r="C521" s="140"/>
       <c r="D521" s="140"/>
       <c r="E521" s="187" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F521" s="193">
         <f>AVERAGE(J521:J525)</f>
         <v>401.60399999999998</v>
       </c>
       <c r="G521" s="140" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H521" s="194">
         <v>42408</v>
       </c>
-      <c r="I521" s="237">
+      <c r="I521" s="223">
         <v>1</v>
       </c>
-      <c r="J521" s="238">
+      <c r="J521" s="224">
         <v>395.65</v>
       </c>
-      <c r="K521" s="239">
+      <c r="K521" s="225">
         <v>1420</v>
       </c>
       <c r="L521" s="140"/>
@@ -16108,25 +16250,25 @@
       <c r="C522" s="140"/>
       <c r="D522" s="140"/>
       <c r="E522" s="187" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F522" s="195">
         <f>F521/1000</f>
         <v>0.40160399999999996</v>
       </c>
       <c r="G522" s="140" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H522" s="194">
         <v>42401</v>
       </c>
-      <c r="I522" s="237">
+      <c r="I522" s="223">
         <v>1</v>
       </c>
-      <c r="J522" s="238">
+      <c r="J522" s="224">
         <v>399.79</v>
       </c>
-      <c r="K522" s="240">
+      <c r="K522" s="226">
         <v>1425</v>
       </c>
       <c r="L522" s="140"/>
@@ -16152,13 +16294,13 @@
       <c r="H523" s="194">
         <v>42394</v>
       </c>
-      <c r="I523" s="237">
+      <c r="I523" s="223">
         <v>1</v>
       </c>
-      <c r="J523" s="238">
+      <c r="J523" s="224">
         <v>393.17</v>
       </c>
-      <c r="K523" s="240">
+      <c r="K523" s="226">
         <v>1417</v>
       </c>
       <c r="L523" s="140"/>
@@ -16178,28 +16320,28 @@
       <c r="B524" s="188"/>
       <c r="C524" s="140"/>
       <c r="D524" s="140" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E524" s="187" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F524" s="193">
         <f>AVERAGE(K521:K525)</f>
         <v>1427.2</v>
       </c>
       <c r="G524" s="140" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H524" s="194">
         <v>42387</v>
       </c>
-      <c r="I524" s="237">
+      <c r="I524" s="223">
         <v>1</v>
       </c>
-      <c r="J524" s="238">
+      <c r="J524" s="224">
         <v>402.27</v>
       </c>
-      <c r="K524" s="240">
+      <c r="K524" s="226">
         <v>1428</v>
       </c>
       <c r="L524" s="140"/>
@@ -16220,25 +16362,25 @@
       <c r="C525" s="140"/>
       <c r="D525" s="140"/>
       <c r="E525" s="187" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F525" s="195">
         <f>F524/1000</f>
         <v>1.4272</v>
       </c>
       <c r="G525" s="140" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H525" s="194">
         <v>42380</v>
       </c>
-      <c r="I525" s="237">
+      <c r="I525" s="223">
         <v>1</v>
       </c>
-      <c r="J525" s="238">
+      <c r="J525" s="224">
         <v>417.14</v>
       </c>
-      <c r="K525" s="240">
+      <c r="K525" s="226">
         <v>1446</v>
       </c>
       <c r="L525" s="140"/>
@@ -16264,13 +16406,13 @@
       <c r="H526" s="194">
         <v>42373</v>
       </c>
-      <c r="I526" s="237">
+      <c r="I526" s="223">
         <v>1</v>
       </c>
-      <c r="J526" s="238">
+      <c r="J526" s="224">
         <v>412.18</v>
       </c>
-      <c r="K526" s="240">
+      <c r="K526" s="226">
         <v>1440</v>
       </c>
       <c r="L526" s="140"/>
@@ -16290,7 +16432,7 @@
       <c r="B527" s="188"/>
       <c r="C527" s="140"/>
       <c r="D527" s="143" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E527" s="140"/>
       <c r="F527" s="198"/>
@@ -16298,13 +16440,13 @@
       <c r="H527" s="194">
         <v>42352</v>
       </c>
-      <c r="I527" s="237">
+      <c r="I527" s="223">
         <v>1</v>
       </c>
-      <c r="J527" s="238">
+      <c r="J527" s="224">
         <v>435.02</v>
       </c>
-      <c r="K527" s="240">
+      <c r="K527" s="226">
         <v>1463</v>
       </c>
       <c r="L527" s="140"/>
@@ -16324,27 +16466,27 @@
       <c r="B528" s="188"/>
       <c r="C528" s="140"/>
       <c r="D528" s="140" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E528" s="187" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F528" s="140">
         <v>21</v>
       </c>
       <c r="G528" s="140" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H528" s="194">
         <v>42345</v>
       </c>
-      <c r="I528" s="237">
+      <c r="I528" s="223">
         <v>1</v>
       </c>
-      <c r="J528" s="238">
+      <c r="J528" s="224">
         <v>452.38</v>
       </c>
-      <c r="K528" s="240">
+      <c r="K528" s="226">
         <v>1484</v>
       </c>
       <c r="L528" s="140"/>
@@ -16364,28 +16506,28 @@
       <c r="B529" s="188"/>
       <c r="C529" s="140"/>
       <c r="D529" s="140" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E529" s="187" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F529" s="140">
         <f>766.07/1000</f>
         <v>0.76607000000000003</v>
       </c>
       <c r="G529" s="140" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H529" s="194">
         <v>42338</v>
       </c>
-      <c r="I529" s="237">
+      <c r="I529" s="223">
         <v>1</v>
       </c>
-      <c r="J529" s="238">
+      <c r="J529" s="224">
         <v>459.81</v>
       </c>
-      <c r="K529" s="240">
+      <c r="K529" s="226">
         <v>1493</v>
       </c>
       <c r="L529" s="140"/>
@@ -16405,28 +16547,28 @@
       <c r="B530" s="188"/>
       <c r="C530" s="140"/>
       <c r="D530" s="140" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E530" s="187" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F530" s="198">
         <f>8/1000</f>
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="G530" s="140" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H530" s="194">
         <v>42331</v>
       </c>
-      <c r="I530" s="237">
+      <c r="I530" s="223">
         <v>1</v>
       </c>
-      <c r="J530" s="238">
+      <c r="J530" s="224">
         <v>469.73</v>
       </c>
-      <c r="K530" s="240">
+      <c r="K530" s="226">
         <v>1505</v>
       </c>
       <c r="L530" s="140"/>
@@ -16452,13 +16594,13 @@
       <c r="H531" s="194">
         <v>42324</v>
       </c>
-      <c r="I531" s="237">
+      <c r="I531" s="223">
         <v>1</v>
       </c>
-      <c r="J531" s="238">
+      <c r="J531" s="224">
         <v>492.87</v>
       </c>
-      <c r="K531" s="240">
+      <c r="K531" s="226">
         <v>1533</v>
       </c>
       <c r="L531" s="140"/>
@@ -16478,28 +16620,28 @@
       <c r="B532" s="188"/>
       <c r="C532" s="140"/>
       <c r="D532" s="140" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E532" s="187" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F532" s="198">
         <f>(F530+F529+F522)*1.21</f>
         <v>1.4225655399999999</v>
       </c>
       <c r="G532" s="140" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H532" s="194">
         <v>42317</v>
       </c>
-      <c r="I532" s="237">
+      <c r="I532" s="223">
         <v>1</v>
       </c>
-      <c r="J532" s="238">
+      <c r="J532" s="224">
         <v>478</v>
       </c>
-      <c r="K532" s="240">
+      <c r="K532" s="226">
         <v>1515</v>
       </c>
       <c r="L532" s="140"/>
@@ -16525,13 +16667,13 @@
       <c r="H533" s="194">
         <v>42310</v>
       </c>
-      <c r="I533" s="237">
+      <c r="I533" s="223">
         <v>1</v>
       </c>
-      <c r="J533" s="238">
+      <c r="J533" s="224">
         <v>449.07</v>
       </c>
-      <c r="K533" s="240">
+      <c r="K533" s="226">
         <v>1480</v>
       </c>
       <c r="L533" s="140"/>
@@ -16557,13 +16699,13 @@
       <c r="H534" s="194">
         <v>42303</v>
       </c>
-      <c r="I534" s="237">
+      <c r="I534" s="223">
         <v>1</v>
       </c>
-      <c r="J534" s="238">
+      <c r="J534" s="224">
         <v>439.98</v>
       </c>
-      <c r="K534" s="240">
+      <c r="K534" s="226">
         <v>1469</v>
       </c>
       <c r="L534" s="140"/>
@@ -16589,13 +16731,13 @@
       <c r="H535" s="194">
         <v>42296</v>
       </c>
-      <c r="I535" s="237">
+      <c r="I535" s="223">
         <v>1</v>
       </c>
-      <c r="J535" s="238">
+      <c r="J535" s="224">
         <v>454.03</v>
       </c>
-      <c r="K535" s="240">
+      <c r="K535" s="226">
         <v>1486</v>
       </c>
       <c r="L535" s="140"/>
@@ -16621,13 +16763,13 @@
       <c r="H536" s="194">
         <v>42289</v>
       </c>
-      <c r="I536" s="237">
+      <c r="I536" s="223">
         <v>1</v>
       </c>
-      <c r="J536" s="238">
+      <c r="J536" s="224">
         <v>462.29</v>
       </c>
-      <c r="K536" s="240">
+      <c r="K536" s="226">
         <v>1496</v>
       </c>
       <c r="L536" s="140"/>
@@ -16653,13 +16795,13 @@
       <c r="H537" s="194">
         <v>42282</v>
       </c>
-      <c r="I537" s="237">
+      <c r="I537" s="223">
         <v>1</v>
       </c>
-      <c r="J537" s="238">
+      <c r="J537" s="224">
         <v>451.55</v>
       </c>
-      <c r="K537" s="240">
+      <c r="K537" s="226">
         <v>1483</v>
       </c>
       <c r="L537" s="140"/>
@@ -16685,13 +16827,13 @@
       <c r="H538" s="194">
         <v>42275</v>
       </c>
-      <c r="I538" s="237">
+      <c r="I538" s="223">
         <v>1</v>
       </c>
-      <c r="J538" s="238">
+      <c r="J538" s="224">
         <v>463.12</v>
       </c>
-      <c r="K538" s="240">
+      <c r="K538" s="226">
         <v>1497</v>
       </c>
       <c r="L538" s="140"/>
@@ -16717,13 +16859,13 @@
       <c r="H539" s="194">
         <v>42268</v>
       </c>
-      <c r="I539" s="237">
+      <c r="I539" s="223">
         <v>1</v>
       </c>
-      <c r="J539" s="238">
+      <c r="J539" s="224">
         <v>472.21</v>
       </c>
-      <c r="K539" s="240">
+      <c r="K539" s="226">
         <v>1508</v>
       </c>
       <c r="L539" s="140"/>
@@ -16749,13 +16891,13 @@
       <c r="H540" s="194">
         <v>42261</v>
       </c>
-      <c r="I540" s="237">
+      <c r="I540" s="223">
         <v>1</v>
       </c>
-      <c r="J540" s="238">
+      <c r="J540" s="224">
         <v>481.3</v>
       </c>
-      <c r="K540" s="240">
+      <c r="K540" s="226">
         <v>1519</v>
       </c>
       <c r="L540" s="187"/>
@@ -16781,13 +16923,13 @@
       <c r="H541" s="194">
         <v>42254</v>
       </c>
-      <c r="I541" s="237">
+      <c r="I541" s="223">
         <v>1</v>
       </c>
-      <c r="J541" s="238">
+      <c r="J541" s="224">
         <v>482.13</v>
       </c>
-      <c r="K541" s="240">
+      <c r="K541" s="226">
         <v>1520</v>
       </c>
       <c r="L541" s="187"/>
@@ -16813,13 +16955,13 @@
       <c r="H542" s="194">
         <v>42247</v>
       </c>
-      <c r="I542" s="237">
+      <c r="I542" s="223">
         <v>1</v>
       </c>
-      <c r="J542" s="238">
+      <c r="J542" s="224">
         <v>482.95</v>
       </c>
-      <c r="K542" s="240">
+      <c r="K542" s="226">
         <v>1521</v>
       </c>
       <c r="L542" s="187"/>
@@ -16845,13 +16987,13 @@
       <c r="H543" s="194">
         <v>42240</v>
       </c>
-      <c r="I543" s="237">
+      <c r="I543" s="223">
         <v>1</v>
       </c>
-      <c r="J543" s="238">
+      <c r="J543" s="224">
         <v>513.53</v>
       </c>
-      <c r="K543" s="240">
+      <c r="K543" s="226">
         <v>1558</v>
       </c>
       <c r="L543" s="187"/>
@@ -16877,13 +17019,13 @@
       <c r="H544" s="194">
         <v>42233</v>
       </c>
-      <c r="I544" s="237">
+      <c r="I544" s="223">
         <v>1</v>
       </c>
-      <c r="J544" s="238">
+      <c r="J544" s="224">
         <v>542.46</v>
       </c>
-      <c r="K544" s="240">
+      <c r="K544" s="226">
         <v>1593</v>
       </c>
       <c r="L544" s="187"/>
@@ -16909,13 +17051,13 @@
       <c r="H545" s="194">
         <v>42226</v>
       </c>
-      <c r="I545" s="237">
+      <c r="I545" s="223">
         <v>1</v>
       </c>
-      <c r="J545" s="238">
+      <c r="J545" s="224">
         <v>562.29</v>
       </c>
-      <c r="K545" s="240">
+      <c r="K545" s="226">
         <v>1617</v>
       </c>
       <c r="L545" s="187"/>
@@ -16941,13 +17083,13 @@
       <c r="H546" s="194">
         <v>42219</v>
       </c>
-      <c r="I546" s="237">
+      <c r="I546" s="223">
         <v>1</v>
       </c>
-      <c r="J546" s="238">
+      <c r="J546" s="224">
         <v>573.86</v>
       </c>
-      <c r="K546" s="240">
+      <c r="K546" s="226">
         <v>1631</v>
       </c>
       <c r="L546" s="187"/>
@@ -16973,13 +17115,13 @@
       <c r="H547" s="194">
         <v>42212</v>
       </c>
-      <c r="I547" s="237">
+      <c r="I547" s="223">
         <v>1</v>
       </c>
-      <c r="J547" s="238">
+      <c r="J547" s="224">
         <v>586.26</v>
       </c>
-      <c r="K547" s="240">
+      <c r="K547" s="226">
         <v>1646</v>
       </c>
       <c r="L547" s="187"/>
@@ -17005,13 +17147,13 @@
       <c r="H548" s="194">
         <v>42205</v>
       </c>
-      <c r="I548" s="237">
+      <c r="I548" s="223">
         <v>1</v>
       </c>
-      <c r="J548" s="238">
+      <c r="J548" s="224">
         <v>599.48</v>
       </c>
-      <c r="K548" s="240">
+      <c r="K548" s="226">
         <v>1662</v>
       </c>
       <c r="L548" s="187"/>
@@ -17037,13 +17179,13 @@
       <c r="H549" s="194">
         <v>42198</v>
       </c>
-      <c r="I549" s="237">
+      <c r="I549" s="223">
         <v>1</v>
       </c>
-      <c r="J549" s="238">
+      <c r="J549" s="224">
         <v>617.66999999999996</v>
       </c>
-      <c r="K549" s="240">
+      <c r="K549" s="226">
         <v>1684</v>
       </c>
       <c r="L549" s="187"/>
@@ -17069,13 +17211,13 @@
       <c r="H550" s="194">
         <v>42191</v>
       </c>
-      <c r="I550" s="237">
+      <c r="I550" s="223">
         <v>1</v>
       </c>
-      <c r="J550" s="238">
+      <c r="J550" s="224">
         <v>601.14</v>
       </c>
-      <c r="K550" s="240">
+      <c r="K550" s="226">
         <v>1664</v>
       </c>
       <c r="L550" s="187"/>
@@ -17148,7 +17290,7 @@
     <row r="558" spans="1:25" customFormat="1" ht="16">
       <c r="B558" s="127"/>
       <c r="C558" s="126" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D558" s="140"/>
       <c r="E558" s="140"/>
@@ -17182,22 +17324,22 @@
     <row r="561" spans="2:8">
       <c r="B561" s="127"/>
       <c r="D561" s="184" t="s">
+        <v>148</v>
+      </c>
+      <c r="F561" s="184" t="s">
         <v>149</v>
       </c>
-      <c r="F561" s="184" t="s">
+      <c r="G561" s="184" t="s">
         <v>150</v>
-      </c>
-      <c r="G561" s="184" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="562" spans="2:8">
       <c r="B562" s="127"/>
       <c r="D562" s="199" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G562" s="184" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="563" spans="2:8">
@@ -17209,10 +17351,10 @@
         <v>0.6</v>
       </c>
       <c r="G564" s="199" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H564" s="199" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="565" spans="2:8">
@@ -17222,10 +17364,10 @@
         <v>1.4272</v>
       </c>
       <c r="G565" s="199" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H565" s="199" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="566" spans="2:8">
@@ -17235,10 +17377,10 @@
         <v>2.0272000000000001</v>
       </c>
       <c r="G566" s="199" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H566" s="199" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="567" spans="2:8">
@@ -17251,10 +17393,10 @@
         <v>0.76607000000000003</v>
       </c>
       <c r="G568" s="199" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H568" s="199" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="569" spans="2:8">
@@ -17264,10 +17406,10 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="G569" s="199" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H569" s="199" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="570" spans="2:8">
@@ -17277,10 +17419,10 @@
         <v>21</v>
       </c>
       <c r="G570" s="199" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H570" s="199" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="571" spans="2:8">
@@ -17306,10 +17448,10 @@
         <v>0.90130190082644646</v>
       </c>
       <c r="G575" s="199" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H575" s="199" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="576" spans="2:8">

</xml_diff>